<commit_message>
Created request report and refactoring several parts of code. Added mocks and test for new report.
</commit_message>
<xml_diff>
--- a/reports/assets/templates/xlsx/template.xlsx
+++ b/reports/assets/templates/xlsx/template.xlsx
@@ -5,22 +5,125 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\canuarb00\Desktop\Connectors\connect-reports\connect_reports\reports\test_report\templates\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\canuarb00\Desktop\Connectors\adobe-reports\reports\assets\templates\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C44C717B-2D59-4E0C-BB62-15D84F78C896}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78EB1FDA-FEE7-43C2-A4CE-221790D69F59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="735" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$AG$1</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+  <si>
+    <t>Asset Id</t>
+  </si>
+  <si>
+    <t>Asset Status</t>
+  </si>
+  <si>
+    <t>External Id</t>
+  </si>
+  <si>
+    <t>Product Id</t>
+  </si>
+  <si>
+    <t>Provider Id</t>
+  </si>
+  <si>
+    <t>Provider Name</t>
+  </si>
+  <si>
+    <t>Marketplace Id</t>
+  </si>
+  <si>
+    <t>Marketplace Name</t>
+  </si>
+  <si>
+    <t>Contract Id</t>
+  </si>
+  <si>
+    <t>Contract Name</t>
+  </si>
+  <si>
+    <t>Reseller Id</t>
+  </si>
+  <si>
+    <t>Reseller External Id</t>
+  </si>
+  <si>
+    <t>Reseller Name</t>
+  </si>
+  <si>
+    <t>Created At</t>
+  </si>
+  <si>
+    <t>Customer Id</t>
+  </si>
+  <si>
+    <t>Customer External Id</t>
+  </si>
+  <si>
+    <t>Customer Name</t>
+  </si>
+  <si>
+    <t>Seamless Move</t>
+  </si>
+  <si>
+    <t>Discount Group</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Renewal Date</t>
+  </si>
+  <si>
+    <t>PurchaseType</t>
+  </si>
+  <si>
+    <t>Adobe Customer Id</t>
+  </si>
+  <si>
+    <t>Adobe VIP Number</t>
+  </si>
+  <si>
+    <t>Adobe User Email</t>
+  </si>
+  <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>Reseller Cost</t>
+  </si>
+  <si>
+    <t>MSRP</t>
+  </si>
+  <si>
+    <t>Seats</t>
+  </si>
+  <si>
+    <t>USD Cost</t>
+  </si>
+  <si>
+    <t>USD Reseller Cost</t>
+  </si>
+  <si>
+    <t>USD MSRP</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -34,15 +137,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -50,12 +159,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -358,14 +485,152 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:AG1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5:H5"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="2" max="2" width="13.6328125" customWidth="1"/>
+    <col min="3" max="3" width="12.7265625" customWidth="1"/>
+    <col min="4" max="4" width="11.26953125" customWidth="1"/>
+    <col min="5" max="5" width="13.6328125" customWidth="1"/>
+    <col min="6" max="6" width="18.81640625" customWidth="1"/>
+    <col min="7" max="7" width="13.90625" customWidth="1"/>
+    <col min="8" max="8" width="18.81640625" customWidth="1"/>
+    <col min="9" max="9" width="12.90625" customWidth="1"/>
+    <col min="10" max="10" width="15.26953125" customWidth="1"/>
+    <col min="11" max="11" width="13.1796875" customWidth="1"/>
+    <col min="12" max="12" width="19.08984375" customWidth="1"/>
+    <col min="13" max="13" width="13.81640625" customWidth="1"/>
+    <col min="14" max="14" width="12.90625" customWidth="1"/>
+    <col min="15" max="15" width="13.90625" customWidth="1"/>
+    <col min="16" max="16" width="20.7265625" customWidth="1"/>
+    <col min="17" max="17" width="14.453125" customWidth="1"/>
+    <col min="18" max="18" width="13.453125" customWidth="1"/>
+    <col min="19" max="19" width="14.81640625" customWidth="1"/>
+    <col min="20" max="20" width="10.36328125" customWidth="1"/>
+    <col min="21" max="21" width="13.36328125" customWidth="1"/>
+    <col min="22" max="22" width="15.36328125" customWidth="1"/>
+    <col min="23" max="23" width="18.36328125" customWidth="1"/>
+    <col min="24" max="24" width="19.81640625" customWidth="1"/>
+    <col min="25" max="25" width="17.08984375" customWidth="1"/>
+    <col min="26" max="26" width="11.453125" customWidth="1"/>
+    <col min="27" max="27" width="11" customWidth="1"/>
+    <col min="28" max="28" width="13.7265625" customWidth="1"/>
+    <col min="29" max="29" width="10.90625" customWidth="1"/>
+    <col min="30" max="30" width="10" customWidth="1"/>
+    <col min="31" max="31" width="13.6328125" customWidth="1"/>
+    <col min="32" max="32" width="16.6328125" customWidth="1"/>
+    <col min="33" max="33" width="13.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:AG1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Pull request #11: CAD-1153 include the filters and templates to show the 3YC assets and request
Merge in SITC/adobe-reports from CAD-1153-p1-find-in-the-active-assets-reports-the-new-columns to master

Squashed commit of the following:

commit 69174ce336cb2cd9b674f2b47bb45b94449c74c3
Author: David Franco <david.franco@cloublue.com>
Date:   Thu Aug 17 16:51:22 2023 +0200

    CAD-1153 improve test coverage

commit 7dbd3a53b3c7251ef5c5cead2a0a28a70e7d6337
Author: David Franco <david.franco@cloublue.com>
Date:   Thu Aug 17 13:56:25 2023 +0200

    CAD-1153 improve the test coverage

commit f173a708e35dcb63b6bf419995fd98ed1d458c95
Author: David Franco <david.franco@cloublue.com>
Date:   Thu Aug 17 13:42:11 2023 +0200

    CAD-1153 correct the test

commit 167d06753ba8acccb8e5a5b63b9e72da10495abd
Author: David Franco <david.franco@cloublue.com>
Date:   Thu Aug 17 13:32:38 2023 +0200

    CAD-1153 include the filters and templates to show the 3YC assets and request
</commit_message>
<xml_diff>
--- a/reports/assets/templates/xlsx/template.xlsx
+++ b/reports/assets/templates/xlsx/template.xlsx
@@ -1,29 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\canuarb00\Desktop\Connectors\adobe-reports\reports\assets\templates\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dfranco00/Sites/adobe-reports/reports/assets/templates/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78EB1FDA-FEE7-43C2-A4CE-221790D69F59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3703DC5-15F6-C34B-A6E7-4B3FF7757F96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$AG$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$AJ$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Asset Id</t>
   </si>
@@ -122,6 +122,15 @@
   </si>
   <si>
     <t>USD MSRP</t>
+  </si>
+  <si>
+    <t>commitment</t>
+  </si>
+  <si>
+    <t>commitment start date</t>
+  </si>
+  <si>
+    <t>commitment end date</t>
   </si>
 </sst>
 </file>
@@ -485,50 +494,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AG1"/>
+  <dimension ref="A1:AJ1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="AC9" sqref="AC9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="13.6328125" customWidth="1"/>
-    <col min="3" max="3" width="12.7265625" customWidth="1"/>
-    <col min="4" max="4" width="11.26953125" customWidth="1"/>
-    <col min="5" max="5" width="13.6328125" customWidth="1"/>
-    <col min="6" max="6" width="18.81640625" customWidth="1"/>
-    <col min="7" max="7" width="13.90625" customWidth="1"/>
-    <col min="8" max="8" width="18.81640625" customWidth="1"/>
-    <col min="9" max="9" width="12.90625" customWidth="1"/>
-    <col min="10" max="10" width="15.26953125" customWidth="1"/>
-    <col min="11" max="11" width="13.1796875" customWidth="1"/>
-    <col min="12" max="12" width="19.08984375" customWidth="1"/>
-    <col min="13" max="13" width="13.81640625" customWidth="1"/>
-    <col min="14" max="14" width="12.90625" customWidth="1"/>
-    <col min="15" max="15" width="13.90625" customWidth="1"/>
-    <col min="16" max="16" width="20.7265625" customWidth="1"/>
-    <col min="17" max="17" width="14.453125" customWidth="1"/>
-    <col min="18" max="18" width="13.453125" customWidth="1"/>
-    <col min="19" max="19" width="14.81640625" customWidth="1"/>
-    <col min="20" max="20" width="10.36328125" customWidth="1"/>
-    <col min="21" max="21" width="13.36328125" customWidth="1"/>
-    <col min="22" max="22" width="15.36328125" customWidth="1"/>
-    <col min="23" max="23" width="18.36328125" customWidth="1"/>
-    <col min="24" max="24" width="19.81640625" customWidth="1"/>
-    <col min="25" max="25" width="17.08984375" customWidth="1"/>
-    <col min="26" max="26" width="11.453125" customWidth="1"/>
-    <col min="27" max="27" width="11" customWidth="1"/>
-    <col min="28" max="28" width="13.7265625" customWidth="1"/>
-    <col min="29" max="29" width="10.90625" customWidth="1"/>
-    <col min="30" max="30" width="10" customWidth="1"/>
-    <col min="31" max="31" width="13.6328125" customWidth="1"/>
-    <col min="32" max="32" width="16.6328125" customWidth="1"/>
-    <col min="33" max="33" width="13.26953125" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" customWidth="1"/>
+    <col min="6" max="6" width="18.83203125" customWidth="1"/>
+    <col min="7" max="7" width="13.83203125" customWidth="1"/>
+    <col min="8" max="8" width="18.83203125" customWidth="1"/>
+    <col min="9" max="9" width="12.83203125" customWidth="1"/>
+    <col min="10" max="10" width="15.33203125" customWidth="1"/>
+    <col min="11" max="11" width="13.1640625" customWidth="1"/>
+    <col min="12" max="12" width="19.1640625" customWidth="1"/>
+    <col min="13" max="13" width="13.83203125" customWidth="1"/>
+    <col min="14" max="14" width="12.83203125" customWidth="1"/>
+    <col min="15" max="15" width="13.83203125" customWidth="1"/>
+    <col min="16" max="16" width="20.6640625" customWidth="1"/>
+    <col min="17" max="17" width="14.5" customWidth="1"/>
+    <col min="18" max="18" width="13.5" customWidth="1"/>
+    <col min="19" max="19" width="14.83203125" customWidth="1"/>
+    <col min="20" max="20" width="10.33203125" customWidth="1"/>
+    <col min="21" max="21" width="13.33203125" customWidth="1"/>
+    <col min="22" max="22" width="15.33203125" customWidth="1"/>
+    <col min="23" max="23" width="18.33203125" customWidth="1"/>
+    <col min="24" max="24" width="19.83203125" customWidth="1"/>
+    <col min="25" max="26" width="17.1640625" customWidth="1"/>
+    <col min="27" max="27" width="23.83203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.5" customWidth="1"/>
+    <col min="30" max="30" width="11" customWidth="1"/>
+    <col min="31" max="31" width="13.6640625" customWidth="1"/>
+    <col min="32" max="32" width="10.83203125" customWidth="1"/>
+    <col min="33" max="33" width="10" customWidth="1"/>
+    <col min="34" max="34" width="13.6640625" customWidth="1"/>
+    <col min="35" max="35" width="16.6640625" customWidth="1"/>
+    <col min="36" max="36" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -605,32 +616,41 @@
         <v>24</v>
       </c>
       <c r="Z1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>32</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AG1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:AJ1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Pull request #13: CAD-1156 add the recommitment columns
Merge in SITC/adobe-reports from CAD-1156-p4-filter-approved-requests-report-to-find-requests-with-3-years-commitment-or-consumables to master

Squashed commit of the following:

commit 0b859212ebca5c17dc84cee3ede7b77472ce898b
Author: David Franco <david.franco@cloublue.com>
Date:   Fri Aug 18 16:33:51 2023 +0200

    CAD-1156 add the recommitment columns
</commit_message>
<xml_diff>
--- a/reports/assets/templates/xlsx/template.xlsx
+++ b/reports/assets/templates/xlsx/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dfranco00/Sites/adobe-reports/reports/assets/templates/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3703DC5-15F6-C34B-A6E7-4B3FF7757F96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BD23EAC-075E-8648-B8D2-3535ACA8C3B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$AJ$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$AN$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Asset Id</t>
   </si>
@@ -131,6 +131,18 @@
   </si>
   <si>
     <t>commitment end date</t>
+  </si>
+  <si>
+    <t>recommitment</t>
+  </si>
+  <si>
+    <t>recommitment start date</t>
+  </si>
+  <si>
+    <t>recommitment end date</t>
+  </si>
+  <si>
+    <t>external reference id</t>
   </si>
 </sst>
 </file>
@@ -494,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AJ1"/>
+  <dimension ref="A1:AN1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="AC9" sqref="AC9"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="R28" sqref="R28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -518,28 +530,30 @@
     <col min="14" max="14" width="12.83203125" customWidth="1"/>
     <col min="15" max="15" width="13.83203125" customWidth="1"/>
     <col min="16" max="16" width="20.6640625" customWidth="1"/>
-    <col min="17" max="17" width="14.5" customWidth="1"/>
-    <col min="18" max="18" width="13.5" customWidth="1"/>
-    <col min="19" max="19" width="14.83203125" customWidth="1"/>
-    <col min="20" max="20" width="10.33203125" customWidth="1"/>
-    <col min="21" max="21" width="13.33203125" customWidth="1"/>
-    <col min="22" max="22" width="15.33203125" customWidth="1"/>
-    <col min="23" max="23" width="18.33203125" customWidth="1"/>
-    <col min="24" max="24" width="19.83203125" customWidth="1"/>
-    <col min="25" max="26" width="17.1640625" customWidth="1"/>
-    <col min="27" max="27" width="23.83203125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="23.1640625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="11.5" customWidth="1"/>
-    <col min="30" max="30" width="11" customWidth="1"/>
-    <col min="31" max="31" width="13.6640625" customWidth="1"/>
-    <col min="32" max="32" width="10.83203125" customWidth="1"/>
-    <col min="33" max="33" width="10" customWidth="1"/>
-    <col min="34" max="34" width="13.6640625" customWidth="1"/>
-    <col min="35" max="35" width="16.6640625" customWidth="1"/>
-    <col min="36" max="36" width="13.33203125" customWidth="1"/>
+    <col min="17" max="17" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.5" customWidth="1"/>
+    <col min="20" max="20" width="14.83203125" customWidth="1"/>
+    <col min="21" max="21" width="10.33203125" customWidth="1"/>
+    <col min="22" max="22" width="13.33203125" customWidth="1"/>
+    <col min="23" max="23" width="15.33203125" customWidth="1"/>
+    <col min="24" max="24" width="18.33203125" customWidth="1"/>
+    <col min="25" max="25" width="19.83203125" customWidth="1"/>
+    <col min="26" max="27" width="17.1640625" customWidth="1"/>
+    <col min="28" max="28" width="23.83203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="32" width="23.1640625" customWidth="1"/>
+    <col min="33" max="33" width="11.5" customWidth="1"/>
+    <col min="34" max="34" width="11" customWidth="1"/>
+    <col min="35" max="35" width="13.6640625" customWidth="1"/>
+    <col min="36" max="36" width="10.83203125" customWidth="1"/>
+    <col min="37" max="37" width="10" customWidth="1"/>
+    <col min="38" max="38" width="13.6640625" customWidth="1"/>
+    <col min="39" max="39" width="16.6640625" customWidth="1"/>
+    <col min="40" max="40" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:40" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -592,65 +606,77 @@
         <v>16</v>
       </c>
       <c r="R1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AG1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>32</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AJ1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:AN1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Pull request #22: CAD-1424: Add Assigne
Merge in SITC/adobe-reports from ~KARLA.NUNEZ/adobe-reports-fork:CAD-1424-add-assignee-and-external_reference_id-columns to master

Squashed commit of the following:

commit 3f846d82f20d6e06be621fee47b260c63db333e1
Author: Karla Nunez <Karla.Nunez@ingrammicro.com>
Date:   Mon Jan 22 09:35:48 2024 +0100

    CAD-1424: Add Assigne
</commit_message>
<xml_diff>
--- a/reports/assets/templates/xlsx/template.xlsx
+++ b/reports/assets/templates/xlsx/template.xlsx
@@ -1,29 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dfranco00/Sites/adobe-reports/reports/assets/templates/xlsx/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\knunez00\Documents\Repositorios\adobe-reports-fork\reports\assets\templates\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BD23EAC-075E-8648-B8D2-3535ACA8C3B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{338FE591-C290-46DF-9C6D-7BAF342CCEE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$AN$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$AO$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Asset Id</t>
   </si>
@@ -143,6 +143,9 @@
   </si>
   <si>
     <t>external reference id</t>
+  </si>
+  <si>
+    <t>Assignee ID</t>
   </si>
 </sst>
 </file>
@@ -506,177 +509,180 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AN1"/>
+  <dimension ref="A1:AO1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="R28" sqref="R28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" customWidth="1"/>
-    <col min="6" max="6" width="18.83203125" customWidth="1"/>
-    <col min="7" max="7" width="13.83203125" customWidth="1"/>
-    <col min="8" max="8" width="18.83203125" customWidth="1"/>
-    <col min="9" max="9" width="12.83203125" customWidth="1"/>
-    <col min="10" max="10" width="15.33203125" customWidth="1"/>
-    <col min="11" max="11" width="13.1640625" customWidth="1"/>
-    <col min="12" max="12" width="19.1640625" customWidth="1"/>
-    <col min="13" max="13" width="13.83203125" customWidth="1"/>
-    <col min="14" max="14" width="12.83203125" customWidth="1"/>
-    <col min="15" max="15" width="13.83203125" customWidth="1"/>
-    <col min="16" max="16" width="20.6640625" customWidth="1"/>
-    <col min="17" max="17" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.5" customWidth="1"/>
-    <col min="20" max="20" width="14.83203125" customWidth="1"/>
-    <col min="21" max="21" width="10.33203125" customWidth="1"/>
-    <col min="22" max="22" width="13.33203125" customWidth="1"/>
-    <col min="23" max="23" width="15.33203125" customWidth="1"/>
-    <col min="24" max="24" width="18.33203125" customWidth="1"/>
-    <col min="25" max="25" width="19.83203125" customWidth="1"/>
-    <col min="26" max="27" width="17.1640625" customWidth="1"/>
-    <col min="28" max="28" width="23.83203125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="23.1640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="32" width="23.1640625" customWidth="1"/>
-    <col min="33" max="33" width="11.5" customWidth="1"/>
-    <col min="34" max="34" width="11" customWidth="1"/>
-    <col min="35" max="35" width="13.6640625" customWidth="1"/>
-    <col min="36" max="36" width="10.83203125" customWidth="1"/>
-    <col min="37" max="37" width="10" customWidth="1"/>
-    <col min="38" max="38" width="13.6640625" customWidth="1"/>
-    <col min="39" max="39" width="16.6640625" customWidth="1"/>
-    <col min="40" max="40" width="13.33203125" customWidth="1"/>
+    <col min="1" max="2" width="12" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" customWidth="1"/>
+    <col min="7" max="7" width="18.85546875" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" customWidth="1"/>
+    <col min="9" max="9" width="18.85546875" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" customWidth="1"/>
+    <col min="11" max="11" width="15.28515625" customWidth="1"/>
+    <col min="12" max="12" width="13.140625" customWidth="1"/>
+    <col min="13" max="13" width="19.140625" customWidth="1"/>
+    <col min="14" max="14" width="13.85546875" customWidth="1"/>
+    <col min="15" max="15" width="12.85546875" customWidth="1"/>
+    <col min="16" max="16" width="13.85546875" customWidth="1"/>
+    <col min="17" max="17" width="20.7109375" customWidth="1"/>
+    <col min="18" max="18" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.42578125" customWidth="1"/>
+    <col min="21" max="21" width="14.85546875" customWidth="1"/>
+    <col min="22" max="22" width="10.28515625" customWidth="1"/>
+    <col min="23" max="23" width="13.28515625" customWidth="1"/>
+    <col min="24" max="24" width="15.28515625" customWidth="1"/>
+    <col min="25" max="25" width="18.28515625" customWidth="1"/>
+    <col min="26" max="26" width="19.85546875" customWidth="1"/>
+    <col min="27" max="28" width="17.140625" customWidth="1"/>
+    <col min="29" max="29" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="33" width="23.140625" customWidth="1"/>
+    <col min="34" max="34" width="11.42578125" customWidth="1"/>
+    <col min="35" max="35" width="11" customWidth="1"/>
+    <col min="36" max="36" width="13.7109375" customWidth="1"/>
+    <col min="37" max="37" width="10.85546875" customWidth="1"/>
+    <col min="38" max="38" width="10" customWidth="1"/>
+    <col min="39" max="39" width="13.7109375" customWidth="1"/>
+    <col min="40" max="40" width="16.7109375" customWidth="1"/>
+    <col min="41" max="41" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:41" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>32</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AN1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:AO1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Pull request #23: CAD-1533: Fix renewal_date error
Merge in SITC/adobe-reports from ~KARLA.NUNEZ/adobe-reports-fork:bugfix/CAD-1533-clone-issues-with-active-assets-report-template-from-adobe-connect-reports to master

Squashed commit of the following:

commit dfeadba65e079267ad3ad305c33af2b7c53e98bd
Author: Karla Nunez <Karla.Nunez@ingrammicro.com>
Date:   Thu Feb 22 14:27:13 2024 +0100

    CAD-1533: Fix renewal_date error
</commit_message>
<xml_diff>
--- a/reports/assets/templates/xlsx/template.xlsx
+++ b/reports/assets/templates/xlsx/template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\knunez00\Documents\Repositorios\adobe-reports-fork\reports\assets\templates\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{338FE591-C290-46DF-9C6D-7BAF342CCEE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FD3A071-C01E-418C-BE17-F701B01EC7C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$AO$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$AN$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Asset Id</t>
   </si>
@@ -143,9 +143,6 @@
   </si>
   <si>
     <t>external reference id</t>
-  </si>
-  <si>
-    <t>Assignee ID</t>
   </si>
 </sst>
 </file>
@@ -509,180 +506,177 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AO1"/>
+  <dimension ref="A1:AN1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" customWidth="1"/>
-    <col min="7" max="7" width="18.85546875" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" customWidth="1"/>
-    <col min="9" max="9" width="18.85546875" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" customWidth="1"/>
-    <col min="11" max="11" width="15.28515625" customWidth="1"/>
-    <col min="12" max="12" width="13.140625" customWidth="1"/>
-    <col min="13" max="13" width="19.140625" customWidth="1"/>
-    <col min="14" max="14" width="13.85546875" customWidth="1"/>
-    <col min="15" max="15" width="12.85546875" customWidth="1"/>
-    <col min="16" max="16" width="13.85546875" customWidth="1"/>
-    <col min="17" max="17" width="20.7109375" customWidth="1"/>
-    <col min="18" max="18" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.42578125" customWidth="1"/>
-    <col min="21" max="21" width="14.85546875" customWidth="1"/>
-    <col min="22" max="22" width="10.28515625" customWidth="1"/>
-    <col min="23" max="23" width="13.28515625" customWidth="1"/>
-    <col min="24" max="24" width="15.28515625" customWidth="1"/>
-    <col min="25" max="25" width="18.28515625" customWidth="1"/>
-    <col min="26" max="26" width="19.85546875" customWidth="1"/>
-    <col min="27" max="28" width="17.140625" customWidth="1"/>
-    <col min="29" max="29" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="31" max="33" width="23.140625" customWidth="1"/>
-    <col min="34" max="34" width="11.42578125" customWidth="1"/>
-    <col min="35" max="35" width="11" customWidth="1"/>
-    <col min="36" max="36" width="13.7109375" customWidth="1"/>
-    <col min="37" max="37" width="10.85546875" customWidth="1"/>
-    <col min="38" max="38" width="10" customWidth="1"/>
-    <col min="39" max="39" width="13.7109375" customWidth="1"/>
-    <col min="40" max="40" width="16.7109375" customWidth="1"/>
-    <col min="41" max="41" width="13.28515625" customWidth="1"/>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" customWidth="1"/>
+    <col min="10" max="10" width="15.28515625" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" customWidth="1"/>
+    <col min="12" max="12" width="19.140625" customWidth="1"/>
+    <col min="13" max="13" width="13.85546875" customWidth="1"/>
+    <col min="14" max="14" width="12.85546875" customWidth="1"/>
+    <col min="15" max="15" width="13.85546875" customWidth="1"/>
+    <col min="16" max="16" width="20.7109375" customWidth="1"/>
+    <col min="17" max="17" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.42578125" customWidth="1"/>
+    <col min="20" max="20" width="14.85546875" customWidth="1"/>
+    <col min="21" max="21" width="10.28515625" customWidth="1"/>
+    <col min="22" max="22" width="13.28515625" customWidth="1"/>
+    <col min="23" max="23" width="15.28515625" customWidth="1"/>
+    <col min="24" max="24" width="18.28515625" customWidth="1"/>
+    <col min="25" max="25" width="19.85546875" customWidth="1"/>
+    <col min="26" max="27" width="17.140625" customWidth="1"/>
+    <col min="28" max="28" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="32" width="23.140625" customWidth="1"/>
+    <col min="33" max="33" width="11.42578125" customWidth="1"/>
+    <col min="34" max="34" width="11" customWidth="1"/>
+    <col min="35" max="35" width="13.7109375" customWidth="1"/>
+    <col min="36" max="36" width="10.85546875" customWidth="1"/>
+    <col min="37" max="37" width="10" customWidth="1"/>
+    <col min="38" max="38" width="13.7109375" customWidth="1"/>
+    <col min="39" max="39" width="16.7109375" customWidth="1"/>
+    <col min="40" max="40" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:40" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AO1" s="1" t="s">
         <v>32</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AO1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:AN1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Pull request #31: CAD-1833 implement the changes to show requested values in the report
Merge in SITC/adobe-reports from ~KARLA.NUNEZ/adobe-reports-fork:CAD-1833-implement-the-changes-to-show-requested-values-in-the-report to master

Squashed commit of the following:

commit 6d15943eb3f08529f54263591c45c0e92711a5cd
Author: Karla Nunez <Karla.Nunez@ingrammicro.com>
Date:   Fri Aug 23 15:09:13 2024 +0200

    CAD:1833: rename

commit 885e54f08ee558e7853c7ee47d51a2f2d57d6929
Author: Karla Nunez <Karla.Nunez@ingrammicro.com>
Date:   Fri Aug 23 15:05:16 2024 +0200

    CAD-11833: Add new colums
</commit_message>
<xml_diff>
--- a/reports/assets/templates/xlsx/template.xlsx
+++ b/reports/assets/templates/xlsx/template.xlsx
@@ -1,29 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\knunez00\Documents\Repositorios\adobe-reports-fork\reports\assets\templates\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FD3A071-C01E-418C-BE17-F701B01EC7C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D516B415-3CEB-46F6-A057-474D5DB84EED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="420" yWindow="1905" windowWidth="28350" windowHeight="9915" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$AN$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$AW$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>Asset Id</t>
   </si>
@@ -143,6 +143,33 @@
   </si>
   <si>
     <t>external reference id</t>
+  </si>
+  <si>
+    <t>Auto Renewal Status</t>
+  </si>
+  <si>
+    <t>Discount Level Consumables</t>
+  </si>
+  <si>
+    <t>Adobe Subscription Details</t>
+  </si>
+  <si>
+    <t>3YC Y/N</t>
+  </si>
+  <si>
+    <t>3YC Committed Licenses</t>
+  </si>
+  <si>
+    <t>3YC Committed Consumables</t>
+  </si>
+  <si>
+    <t>3YC Recommitment Y/N</t>
+  </si>
+  <si>
+    <t>3YC Recommitted Licenses</t>
+  </si>
+  <si>
+    <t>3YC Recommitted Consumables</t>
   </si>
 </sst>
 </file>
@@ -506,10 +533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AN1"/>
+  <dimension ref="A1:AW1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -532,28 +559,28 @@
     <col min="16" max="16" width="20.7109375" customWidth="1"/>
     <col min="17" max="17" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.42578125" customWidth="1"/>
-    <col min="20" max="20" width="14.85546875" customWidth="1"/>
-    <col min="21" max="21" width="10.28515625" customWidth="1"/>
-    <col min="22" max="22" width="13.28515625" customWidth="1"/>
-    <col min="23" max="23" width="15.28515625" customWidth="1"/>
-    <col min="24" max="24" width="18.28515625" customWidth="1"/>
-    <col min="25" max="25" width="19.85546875" customWidth="1"/>
-    <col min="26" max="27" width="17.140625" customWidth="1"/>
-    <col min="28" max="28" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="32" width="23.140625" customWidth="1"/>
-    <col min="33" max="33" width="11.42578125" customWidth="1"/>
-    <col min="34" max="34" width="11" customWidth="1"/>
-    <col min="35" max="35" width="13.7109375" customWidth="1"/>
-    <col min="36" max="36" width="10.85546875" customWidth="1"/>
-    <col min="37" max="37" width="10" customWidth="1"/>
-    <col min="38" max="38" width="13.7109375" customWidth="1"/>
-    <col min="39" max="39" width="16.7109375" customWidth="1"/>
-    <col min="40" max="40" width="13.28515625" customWidth="1"/>
+    <col min="19" max="20" width="13.42578125" customWidth="1"/>
+    <col min="21" max="22" width="14.85546875" customWidth="1"/>
+    <col min="23" max="23" width="10.28515625" customWidth="1"/>
+    <col min="24" max="24" width="13.28515625" customWidth="1"/>
+    <col min="25" max="25" width="15.28515625" customWidth="1"/>
+    <col min="26" max="26" width="18.28515625" customWidth="1"/>
+    <col min="27" max="27" width="19.85546875" customWidth="1"/>
+    <col min="28" max="39" width="17.140625" customWidth="1"/>
+    <col min="40" max="40" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="42" max="44" width="23.140625" customWidth="1"/>
+    <col min="45" max="45" width="11.42578125" customWidth="1"/>
+    <col min="46" max="46" width="11" customWidth="1"/>
+    <col min="47" max="47" width="13.7109375" customWidth="1"/>
+    <col min="48" max="48" width="10.85546875" customWidth="1"/>
+    <col min="49" max="49" width="10" customWidth="1"/>
+    <col min="50" max="50" width="13.7109375" customWidth="1"/>
+    <col min="51" max="51" width="16.7109375" customWidth="1"/>
+    <col min="52" max="52" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:49" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -612,71 +639,99 @@
         <v>17</v>
       </c>
       <c r="T1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="W1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AH1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AM1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>32</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AN1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:AZ1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>